<commit_message>
Added excel version of data
Provided an excel version of data that has the headers with columns, as the csv does not.
</commit_message>
<xml_diff>
--- a/close-approaches.xlsx
+++ b/close-approaches.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J-Gaming\Documents\Asteroid Close Approaches to Earth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Math-Soft\Asteroid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A0637344-17E7-4485-992E-DCCFBB6D59D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88411297-C570-441A-9BA2-B48ADE624485}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="earthapp" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">earthapp!$P$1:$P$503</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">earthapp!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -871,7 +871,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1349,13 +1349,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1710,40 +1707,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R499"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="3"/>
       <c r="C1" t="s">
         <v>277</v>
       </c>
@@ -28854,9 +28850,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
+  <autoFilter ref="A1:R1" xr:uid="{2C3CD7FB-A3B7-4153-9B2A-DAC9D7095CC2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>